<commit_message>
feat: add corrective status registry and standardize unit test patterns
  - Add corrective-status-registry module with full CRUD operations
  - Add 6 new monthly-report use-cases (L3 summary, incidents by day, bugs by parent, etc.)
  - Enhance analytics dashboard with comprehensive L3 analytics
  - Migrate 45+ unit tests from vi.fn() to vitest-mock-extended pattern
  - Add unit tests for categorization-registry, module-registry, and corrective-status-registry
  - Add path aliases for @categorization-registry and @module-registry

  Or a shorter version:

  feat: add corrective status registry and migrate tests to vitest-mock-extended

  - New corrective-status-registry module with CRUD operations
  - New monthly-report L3 analytics use-cases
  - Enhanced analytics dashboard
  - Standardized all unit tests to use mock<T>() and MockProxy<T>
  - Added test coverage for categorization-registry and module-registry
</commit_message>
<xml_diff>
--- a/apps/reports-api/files/EDWarRooms2025.xlsx
+++ b/apps/reports-api/files/EDWarRooms2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcorpbiz.sharepoint.com/sites/SomosBelcorpRevamp-Development/Documentos compartidos/09. Operation/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1577" documentId="11_FCBEA7B812AF3F2BC6B584C3BFED8787170E5B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB98767D-B2B3-4CD0-822F-0997C9ABF147}"/>
+  <xr:revisionPtr revIDLastSave="1815" documentId="11_FCBEA7B812AF3F2BC6B584C3BFED8787170E5B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11DABBA-C767-4927-8421-8540E54788D4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26040" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="-120" windowWidth="26040" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warrooms" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="332">
   <si>
     <t>Application</t>
   </si>
@@ -930,6 +930,9 @@
     <t>Error by change, Resolutor changed to infra</t>
   </si>
   <si>
+    <t>https://confluence.belcorp.biz/x/MX3vDQ</t>
+  </si>
+  <si>
     <t>ALL|C16|APP CEG|BOLSA DE PEDIDO| nO se no visualizan pedidos en bolsa</t>
   </si>
   <si>
@@ -937,6 +940,102 @@
   </si>
   <si>
     <t>https://confluence.belcorp.biz/x/MxLvDQ</t>
+  </si>
+  <si>
+    <t>DO|PROL|-Error en el proceso PROL ACTIVACION BDI2</t>
+  </si>
+  <si>
+    <t>User mistake, It was identified that one of the levels of a program configured in “N per offer configuration” had a duplicate level.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/L33vDQ</t>
+  </si>
+  <si>
+    <t>MX|UNETE 2.0|BURÓ| CS sin consulta crediticia.</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>Bug, A group of zones does not keep a record of inquiries made to the credit buró and are not configured as a Cash Payment Zone.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/pyzvDQ</t>
+  </si>
+  <si>
+    <t>DO| C17| SB| Incentivos| muestra aviso a la CS que no puede seleccionar Incentivo</t>
+  </si>
+  <si>
+    <t>User mistake, Incorrect configuration of the reported contest</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/LX3vDQ</t>
+  </si>
+  <si>
+    <t>DO|C17|SB|FESTIVALES|Oferta no permite agregarse MENSAJE DE ERROR</t>
+  </si>
+  <si>
+    <t>User mistake, A double festival was set up, and the product was also sent from Affinity as part of the Festival.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/2ETvDQ</t>
+  </si>
+  <si>
+    <t>CO|C18|SB|MULTIPEDIDO POSTERIOR| No aparece experiencia de MB Posterior configurada para hoy</t>
+  </si>
+  <si>
+    <t>The ConfiguracionValidacionZona table had a value of 9 days, which was not enough to cover day 20 according to the billing start date.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/g1DvDQ</t>
+  </si>
+  <si>
+    <t>PE|C18|SB|BONIFICACIONES| NO SE PUEDE SELECCIONAR INCENTIVOS C18</t>
+  </si>
+  <si>
+    <t>Consultant identifies incorrect tender; response expected from SSICC team</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/3E3vDQ</t>
+  </si>
+  <si>
+    <t>EC|C18|SB|BONIFICACIONES|: PUNTAJE NO ACTUALIZADO</t>
+  </si>
+  <si>
+    <t>Resolutor changed to SSICC/ODS - The incentive score is not added together.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/K33vDQ</t>
+  </si>
+  <si>
+    <t>PE|C18|SB|PASE DE PEDIDOS|Producto de Televenta tiene distinto precio entre consultoras</t>
+  </si>
+  <si>
+    <t>User mistake, CUV 37043 submitted a manual update with the repetition factor at 0</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/mmfvDQ</t>
+  </si>
+  <si>
+    <t>BO|C17|PROL|PEDIDO NO SE PUEDE RESERVAR SALE ERROR CS 0721286</t>
+  </si>
+  <si>
+    <t>User mistake, The product with the internal warning has a replacement configured, which was out of stock.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/lmfvDQ</t>
+  </si>
+  <si>
+    <t>BO|C17|SB| CS COD 0717399 NO PUEDE RESERVAR - MENSAJE DE ERROR</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/KX3vDQ</t>
+  </si>
+  <si>
+    <t>CR|C16|SB ADMIN|Campaña 202416 CR no disponible en somosbelcorp</t>
+  </si>
+  <si>
+    <t>Resolutor changed to SSICC/ODS -  Campaign 202416 does not exist in the records of the ods.campania table</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1148,11 +1247,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1459,8 +1564,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}" name="Tabla1" displayName="Tabla1" ref="A1:O140" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O140" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}" name="Tabla1" displayName="Tabla1" ref="A1:O152" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O152" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}">
+    <filterColumn colId="1">
+      <filters>
+        <dateGroupItem year="2025" month="11" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O135">
     <sortCondition ref="A1:A135"/>
   </sortState>
@@ -1804,11 +1915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O140"/>
+  <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.149999999999999" customHeight="1"/>
@@ -1884,7 +1995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="2" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -1929,7 +2040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="3" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1974,7 +2085,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="4" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2019,7 +2130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="5" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -2064,7 +2175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="6" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -2109,7 +2220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="7" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -2154,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="8" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
@@ -2199,7 +2310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="9" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -2244,7 +2355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="10" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2289,7 +2400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15" ht="15" hidden="1">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -2334,7 +2445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15">
+    <row r="12" spans="1:15" ht="15" hidden="1">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -2379,7 +2490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15">
+    <row r="13" spans="1:15" ht="15" hidden="1">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -2424,7 +2535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15">
+    <row r="14" spans="1:15" ht="15" hidden="1">
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
@@ -2469,7 +2580,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15">
+    <row r="15" spans="1:15" ht="15" hidden="1">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -2514,7 +2625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15">
+    <row r="16" spans="1:15" ht="15" hidden="1">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
@@ -2559,7 +2670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15">
+    <row r="17" spans="1:14" ht="15" hidden="1">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -2604,7 +2715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14" ht="15" hidden="1">
       <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
@@ -2649,7 +2760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="19" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15">
+    <row r="20" spans="1:14" ht="15" hidden="1">
       <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
@@ -2739,7 +2850,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="21" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
@@ -2784,7 +2895,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15">
+    <row r="22" spans="1:14" ht="15" hidden="1">
       <c r="A22" s="7" t="s">
         <v>61</v>
       </c>
@@ -2829,7 +2940,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15">
+    <row r="23" spans="1:14" ht="15" hidden="1">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2874,7 +2985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15">
+    <row r="24" spans="1:14" ht="15" hidden="1">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
@@ -2919,7 +3030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15">
+    <row r="25" spans="1:14" ht="15" hidden="1">
       <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
@@ -2964,7 +3075,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15">
+    <row r="26" spans="1:14" ht="15" hidden="1">
       <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
@@ -3009,7 +3120,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15">
+    <row r="27" spans="1:14" ht="15" hidden="1">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3054,7 +3165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="28" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
@@ -3099,7 +3210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="29" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>23</v>
       </c>
@@ -3144,7 +3255,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="30" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>61</v>
       </c>
@@ -3189,7 +3300,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="31" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>23</v>
       </c>
@@ -3234,7 +3345,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="32" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
@@ -3279,7 +3390,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="33" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
@@ -3324,7 +3435,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="34" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>23</v>
       </c>
@@ -3369,7 +3480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="35" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A35" s="7" t="s">
         <v>23</v>
       </c>
@@ -3414,7 +3525,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="36" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
@@ -3459,7 +3570,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="37" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A37" s="7" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3615,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="38" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>23</v>
       </c>
@@ -3549,7 +3660,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="39" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
@@ -3594,7 +3705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="40" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>23</v>
       </c>
@@ -3639,7 +3750,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="41" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>23</v>
       </c>
@@ -3684,7 +3795,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="42" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>15</v>
       </c>
@@ -3729,7 +3840,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="43" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>23</v>
       </c>
@@ -3774,7 +3885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="44" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>52</v>
       </c>
@@ -3819,7 +3930,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="45" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>15</v>
       </c>
@@ -3864,7 +3975,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="46" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>52</v>
       </c>
@@ -3909,7 +4020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="47" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
@@ -3954,7 +4065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="48" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>15</v>
       </c>
@@ -3999,7 +4110,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="49" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>23</v>
       </c>
@@ -4044,7 +4155,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="50" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>23</v>
       </c>
@@ -4089,7 +4200,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="51" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>52</v>
       </c>
@@ -4134,7 +4245,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="52" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>15</v>
       </c>
@@ -4179,7 +4290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="53" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A53" s="7" t="s">
         <v>15</v>
       </c>
@@ -4225,7 +4336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="54" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A54" s="7" t="s">
         <v>23</v>
       </c>
@@ -4270,7 +4381,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="55" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A55" s="7" t="s">
         <v>23</v>
       </c>
@@ -4315,7 +4426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="56" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A56" s="7" t="s">
         <v>15</v>
       </c>
@@ -4360,7 +4471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="57" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>23</v>
       </c>
@@ -4405,7 +4516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="58" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A58" s="7" t="s">
         <v>52</v>
       </c>
@@ -4450,7 +4561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="59" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
@@ -4495,7 +4606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="60" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A60" s="7" t="s">
         <v>23</v>
       </c>
@@ -4540,7 +4651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="61" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A61" s="7" t="s">
         <v>15</v>
       </c>
@@ -4585,7 +4696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="62" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A62" s="7" t="s">
         <v>23</v>
       </c>
@@ -4630,7 +4741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="63" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>23</v>
       </c>
@@ -4675,7 +4786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15">
+    <row r="64" spans="1:14" ht="15" hidden="1">
       <c r="A64" s="7" t="s">
         <v>23</v>
       </c>
@@ -4720,7 +4831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15">
+    <row r="65" spans="1:14" ht="15" hidden="1">
       <c r="A65" s="7" t="s">
         <v>61</v>
       </c>
@@ -4765,7 +4876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15">
+    <row r="66" spans="1:14" ht="15" hidden="1">
       <c r="A66" s="7" t="s">
         <v>23</v>
       </c>
@@ -4810,7 +4921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15">
+    <row r="67" spans="1:14" ht="15" hidden="1">
       <c r="A67" s="7" t="s">
         <v>23</v>
       </c>
@@ -4855,7 +4966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="68" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>23</v>
       </c>
@@ -4900,7 +5011,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="69" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A69" s="7" t="s">
         <v>23</v>
       </c>
@@ -4945,7 +5056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15">
+    <row r="70" spans="1:14" ht="15" hidden="1">
       <c r="A70" s="7" t="s">
         <v>23</v>
       </c>
@@ -4990,7 +5101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15">
+    <row r="71" spans="1:14" ht="15" hidden="1">
       <c r="A71" s="7" t="s">
         <v>23</v>
       </c>
@@ -5035,7 +5146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15">
+    <row r="72" spans="1:14" ht="15" hidden="1">
       <c r="A72" s="7" t="s">
         <v>23</v>
       </c>
@@ -5080,7 +5191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15">
+    <row r="73" spans="1:14" ht="15" hidden="1">
       <c r="A73" s="7" t="s">
         <v>15</v>
       </c>
@@ -5125,7 +5236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15">
+    <row r="74" spans="1:14" ht="15" hidden="1">
       <c r="A74" s="7" t="s">
         <v>23</v>
       </c>
@@ -5170,7 +5281,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15">
+    <row r="75" spans="1:14" ht="15" hidden="1">
       <c r="A75" s="7" t="s">
         <v>23</v>
       </c>
@@ -5215,7 +5326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15">
+    <row r="76" spans="1:14" ht="15" hidden="1">
       <c r="A76" s="7" t="s">
         <v>15</v>
       </c>
@@ -5260,7 +5371,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15">
+    <row r="77" spans="1:14" ht="15" hidden="1">
       <c r="A77" s="7" t="s">
         <v>15</v>
       </c>
@@ -5305,7 +5416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15">
+    <row r="78" spans="1:14" ht="15" hidden="1">
       <c r="A78" s="7" t="s">
         <v>15</v>
       </c>
@@ -5350,7 +5461,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="79" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A79" s="7" t="s">
         <v>23</v>
       </c>
@@ -5392,7 +5503,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="80" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A80" s="7" t="s">
         <v>34</v>
       </c>
@@ -5434,7 +5545,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="81" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A81" s="7" t="s">
         <v>15</v>
       </c>
@@ -5476,7 +5587,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="82" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A82" s="7" t="s">
         <v>23</v>
       </c>
@@ -5518,7 +5629,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="83" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A83" s="7" t="s">
         <v>23</v>
       </c>
@@ -5560,7 +5671,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="84" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A84" s="7" t="s">
         <v>15</v>
       </c>
@@ -5602,7 +5713,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="85" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A85" s="7" t="s">
         <v>23</v>
       </c>
@@ -5644,7 +5755,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="86" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A86" s="7" t="s">
         <v>23</v>
       </c>
@@ -5686,7 +5797,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="87" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A87" s="7" t="s">
         <v>23</v>
       </c>
@@ -5728,7 +5839,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="88" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A88" s="18" t="s">
         <v>23</v>
       </c>
@@ -5770,7 +5881,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="89" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A89" s="18" t="s">
         <v>23</v>
       </c>
@@ -5812,7 +5923,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="90" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A90" s="7" t="s">
         <v>15</v>
       </c>
@@ -5854,7 +5965,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="91" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A91" s="7" t="s">
         <v>15</v>
       </c>
@@ -5896,7 +6007,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="92" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A92" s="7" t="s">
         <v>15</v>
       </c>
@@ -5938,7 +6049,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="93" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A93" s="18" t="s">
         <v>23</v>
       </c>
@@ -5980,7 +6091,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="94" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A94" s="7" t="s">
         <v>15</v>
       </c>
@@ -6022,7 +6133,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="95" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A95" s="18" t="s">
         <v>23</v>
       </c>
@@ -6064,7 +6175,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="96" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A96" s="18" t="s">
         <v>23</v>
       </c>
@@ -6106,7 +6217,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="97" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A97" s="18" t="s">
         <v>23</v>
       </c>
@@ -6148,7 +6259,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="98" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A98" s="18" t="s">
         <v>23</v>
       </c>
@@ -6190,7 +6301,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="99" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A99" s="18" t="s">
         <v>23</v>
       </c>
@@ -6232,7 +6343,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="100" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A100" s="18" t="s">
         <v>34</v>
       </c>
@@ -6274,7 +6385,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="101" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A101" s="18" t="s">
         <v>23</v>
       </c>
@@ -6316,7 +6427,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="102" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A102" s="18" t="s">
         <v>23</v>
       </c>
@@ -6358,7 +6469,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="103" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A103" s="18" t="s">
         <v>34</v>
       </c>
@@ -6400,7 +6511,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15">
+    <row r="104" spans="1:14" ht="15" hidden="1">
       <c r="A104" s="18" t="s">
         <v>23</v>
       </c>
@@ -6442,7 +6553,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="15">
+    <row r="105" spans="1:14" ht="15" hidden="1">
       <c r="A105" s="18" t="s">
         <v>23</v>
       </c>
@@ -6484,7 +6595,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="15">
+    <row r="106" spans="1:14" ht="15" hidden="1">
       <c r="A106" s="18" t="s">
         <v>23</v>
       </c>
@@ -6526,7 +6637,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="15">
+    <row r="107" spans="1:14" ht="15" hidden="1">
       <c r="A107" s="18" t="s">
         <v>23</v>
       </c>
@@ -6568,7 +6679,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15">
+    <row r="108" spans="1:14" ht="15" hidden="1">
       <c r="A108" s="18" t="s">
         <v>23</v>
       </c>
@@ -6610,7 +6721,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15">
+    <row r="109" spans="1:14" ht="15" hidden="1">
       <c r="A109" s="7" t="s">
         <v>15</v>
       </c>
@@ -6652,7 +6763,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="15">
+    <row r="110" spans="1:14" ht="15" hidden="1">
       <c r="A110" s="18" t="s">
         <v>34</v>
       </c>
@@ -6694,7 +6805,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15">
+    <row r="111" spans="1:14" ht="15" hidden="1">
       <c r="A111" s="7" t="s">
         <v>15</v>
       </c>
@@ -6739,7 +6850,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="15">
+    <row r="112" spans="1:14" ht="15" hidden="1">
       <c r="A112" s="18" t="s">
         <v>23</v>
       </c>
@@ -6784,7 +6895,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="15">
+    <row r="113" spans="1:15" ht="15" hidden="1">
       <c r="A113" s="18" t="s">
         <v>23</v>
       </c>
@@ -6832,7 +6943,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="15">
+    <row r="114" spans="1:15" ht="15" hidden="1">
       <c r="A114" s="18" t="s">
         <v>23</v>
       </c>
@@ -6877,7 +6988,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="15">
+    <row r="115" spans="1:15" ht="15" hidden="1">
       <c r="A115" s="18" t="s">
         <v>23</v>
       </c>
@@ -6922,7 +7033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="15">
+    <row r="116" spans="1:15" ht="15" hidden="1">
       <c r="A116" s="18" t="s">
         <v>23</v>
       </c>
@@ -6967,7 +7078,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="117" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A117" s="18" t="s">
         <v>23</v>
       </c>
@@ -7015,7 +7126,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="15">
+    <row r="118" spans="1:15" ht="15" hidden="1">
       <c r="A118" s="7" t="s">
         <v>15</v>
       </c>
@@ -7063,7 +7174,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="15">
+    <row r="119" spans="1:15" ht="15" hidden="1">
       <c r="A119" s="7" t="s">
         <v>15</v>
       </c>
@@ -7108,7 +7219,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="15">
+    <row r="120" spans="1:15" ht="15" hidden="1">
       <c r="A120" s="30" t="s">
         <v>23</v>
       </c>
@@ -7156,7 +7267,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="15">
+    <row r="121" spans="1:15" ht="15" hidden="1">
       <c r="A121" s="30" t="s">
         <v>23</v>
       </c>
@@ -7201,7 +7312,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="15">
+    <row r="122" spans="1:15" ht="15" hidden="1">
       <c r="A122" s="18" t="s">
         <v>23</v>
       </c>
@@ -7246,7 +7357,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="123" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A123" s="28" t="s">
         <v>251</v>
       </c>
@@ -7294,7 +7405,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="124" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A124" s="7" t="s">
         <v>15</v>
       </c>
@@ -7342,7 +7453,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="15">
+    <row r="125" spans="1:15" ht="15" hidden="1">
       <c r="A125" s="7" t="s">
         <v>15</v>
       </c>
@@ -7390,7 +7501,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="126" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A126" s="7" t="s">
         <v>15</v>
       </c>
@@ -7435,7 +7546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="127" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A127" s="18" t="s">
         <v>23</v>
       </c>
@@ -7483,7 +7594,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="128" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A128" s="18" t="s">
         <v>23</v>
       </c>
@@ -7531,7 +7642,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="129" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A129" s="18" t="s">
         <v>23</v>
       </c>
@@ -7541,7 +7652,7 @@
       <c r="C129" s="36">
         <v>128089</v>
       </c>
-      <c r="D129" s="41" t="s">
+      <c r="D129" s="40" t="s">
         <v>270</v>
       </c>
       <c r="E129" s="7" t="s">
@@ -7579,7 +7690,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="130" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A130" s="18" t="s">
         <v>23</v>
       </c>
@@ -7627,7 +7738,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="131" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A131" s="18" t="s">
         <v>23</v>
       </c>
@@ -7672,7 +7783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="132" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A132" s="18" t="s">
         <v>23</v>
       </c>
@@ -7717,7 +7828,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="133" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A133" s="18" t="s">
         <v>23</v>
       </c>
@@ -7765,7 +7876,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="134" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A134" s="28" t="s">
         <v>23</v>
       </c>
@@ -7810,7 +7921,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="135" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A135" s="18" t="s">
         <v>34</v>
       </c>
@@ -7855,11 +7966,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="136" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A136" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B136" s="40">
+      <c r="B136" s="19">
         <v>45958</v>
       </c>
       <c r="C136" s="36">
@@ -7900,11 +8011,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="137" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A137" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B137" s="40">
+      <c r="B137" s="19">
         <v>45958</v>
       </c>
       <c r="C137" s="36">
@@ -7945,11 +8056,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="138" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A138" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B138" s="40">
+      <c r="B138" s="19">
         <v>45958</v>
       </c>
       <c r="C138" s="36">
@@ -7994,7 +8105,7 @@
       <c r="A139" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B139" s="40">
+      <c r="B139" s="19">
         <v>45965</v>
       </c>
       <c r="C139" s="36">
@@ -8033,20 +8144,23 @@
       </c>
       <c r="N139" s="7" t="s">
         <v>46</v>
+      </c>
+      <c r="O139" s="26" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16.149999999999999" customHeight="1">
       <c r="A140" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B140" s="40">
+      <c r="B140" s="19">
         <v>45966</v>
       </c>
       <c r="C140" s="36">
         <v>136341</v>
       </c>
       <c r="D140" s="35" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>17</v>
@@ -8074,14 +8188,545 @@
         <v>20</v>
       </c>
       <c r="M140" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N140" s="7" t="s">
         <v>221</v>
       </c>
       <c r="O140" s="26" t="s">
-        <v>298</v>
-      </c>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A141" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="19">
+        <v>45971</v>
+      </c>
+      <c r="C141" s="36">
+        <v>137357</v>
+      </c>
+      <c r="D141" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" s="10">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="G141" s="7">
+        <v>105</v>
+      </c>
+      <c r="H141" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="I141" s="7">
+        <v>7</v>
+      </c>
+      <c r="J141" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K141" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M141" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="N141" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O141" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A142" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B142" s="19">
+        <v>45973</v>
+      </c>
+      <c r="C142" s="36">
+        <v>138367</v>
+      </c>
+      <c r="D142" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="E142" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F142" s="10">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="G142" s="7">
+        <v>240</v>
+      </c>
+      <c r="H142" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="I142" s="7">
+        <v>15</v>
+      </c>
+      <c r="J142" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K142" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L142" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M142" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="N142" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O142" s="26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A143" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" s="19">
+        <v>45974</v>
+      </c>
+      <c r="C143" s="41">
+        <v>138895</v>
+      </c>
+      <c r="D143" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F143" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G143" s="7">
+        <v>150</v>
+      </c>
+      <c r="H143" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="I143" s="7">
+        <v>6</v>
+      </c>
+      <c r="J143" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L143" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M143" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="N143" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O143" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A144" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" s="19">
+        <v>45981</v>
+      </c>
+      <c r="C144" s="36">
+        <v>139556</v>
+      </c>
+      <c r="D144" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F144" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G144" s="7">
+        <v>160</v>
+      </c>
+      <c r="H144" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="I144" s="7">
+        <v>9</v>
+      </c>
+      <c r="J144" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K144" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L144" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M144" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="N144" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O144" s="37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A145" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B145" s="19">
+        <v>45981</v>
+      </c>
+      <c r="C145" s="36">
+        <v>140551</v>
+      </c>
+      <c r="D145" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F145" s="10">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="G145" s="7">
+        <v>210</v>
+      </c>
+      <c r="H145" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.76388888888888895</v>
+      </c>
+      <c r="I145" s="7">
+        <v>13</v>
+      </c>
+      <c r="J145" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M145" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="N145" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O145" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A146" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B146" s="19">
+        <v>45985</v>
+      </c>
+      <c r="C146" s="36">
+        <v>141251</v>
+      </c>
+      <c r="D146" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F146" s="10">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="G146" s="7">
+        <v>175</v>
+      </c>
+      <c r="H146" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.53125</v>
+      </c>
+      <c r="I146" s="7">
+        <v>12</v>
+      </c>
+      <c r="J146" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K146" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L146" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M146" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="N146" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O146" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A147" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" s="19">
+        <v>45986</v>
+      </c>
+      <c r="C147" s="36">
+        <v>141984</v>
+      </c>
+      <c r="D147" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F147" s="10">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G147" s="7">
+        <v>50</v>
+      </c>
+      <c r="H147" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.83680555555555558</v>
+      </c>
+      <c r="I147" s="7">
+        <v>5</v>
+      </c>
+      <c r="J147" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K147" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L147" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M147" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="N147" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O147" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A148" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B148" s="42">
+        <v>45987</v>
+      </c>
+      <c r="C148" s="36">
+        <v>142358</v>
+      </c>
+      <c r="D148" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F148" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G148" s="7">
+        <v>50</v>
+      </c>
+      <c r="H148" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="I148" s="7">
+        <v>4</v>
+      </c>
+      <c r="J148" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K148" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L148" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M148" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="N148" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O148" s="26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A149" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B149" s="42">
+        <v>45989</v>
+      </c>
+      <c r="C149" s="36">
+        <v>142948</v>
+      </c>
+      <c r="D149" t="s">
+        <v>325</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F149" s="10">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G149" s="7">
+        <v>70</v>
+      </c>
+      <c r="H149" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I149" s="7">
+        <v>6</v>
+      </c>
+      <c r="J149" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M149" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N149" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O149" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A150" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B150" s="42">
+        <v>45989</v>
+      </c>
+      <c r="C150" s="36">
+        <v>142966</v>
+      </c>
+      <c r="D150" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F150" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G150" s="7">
+        <v>65</v>
+      </c>
+      <c r="H150" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="I150" s="7">
+        <v>8</v>
+      </c>
+      <c r="J150" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M150" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N150" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O150" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
+      <c r="A151" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="42">
+        <v>45994</v>
+      </c>
+      <c r="C151" s="36">
+        <v>144540</v>
+      </c>
+      <c r="D151" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F151" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="G151" s="7">
+        <v>35</v>
+      </c>
+      <c r="H151" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.71180555555555558</v>
+      </c>
+      <c r="I151" s="7">
+        <v>12</v>
+      </c>
+      <c r="J151" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K151" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M151" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="N151" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
+      <c r="A152" s="28"/>
+      <c r="B152" s="42"/>
+      <c r="C152" s="43"/>
+      <c r="F152" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8256,33 +8901,40 @@
     <hyperlink ref="C139" r:id="rId169" display="136040" xr:uid="{F80D565B-B60C-432B-B5E5-A8D4B680A58A}"/>
     <hyperlink ref="C140" r:id="rId170" display="136341" xr:uid="{A2DA186D-87E9-49EB-A8D4-844EFEF3E0BC}"/>
     <hyperlink ref="O140" r:id="rId171" xr:uid="{73E6D2D9-56BF-485D-AC48-A46E59BCA29A}"/>
+    <hyperlink ref="C141" r:id="rId172" display="137357" xr:uid="{641393F9-91E6-41F8-9FC9-AEF2EB5CCFA5}"/>
+    <hyperlink ref="C142" r:id="rId173" display="138367" xr:uid="{0BBFBABF-045E-43A3-9668-881698CD6281}"/>
+    <hyperlink ref="C143" r:id="rId174" display="138895" xr:uid="{5E323059-89CB-4C7C-A1B3-B288E2F62593}"/>
+    <hyperlink ref="C144" r:id="rId175" display="139556" xr:uid="{8B91B6CF-93A5-471F-9B80-6E3CE24578C0}"/>
+    <hyperlink ref="O144" r:id="rId176" xr:uid="{0815C2D1-F220-4592-9369-C67917B4D98F}"/>
+    <hyperlink ref="C145" r:id="rId177" display="140551" xr:uid="{374FBAB6-0BA4-4063-9DAC-8FB8296334B4}"/>
+    <hyperlink ref="C146" r:id="rId178" display="141251" xr:uid="{0BF9A3AC-0A07-4ABE-83F2-7BAE5BBE750B}"/>
+    <hyperlink ref="C147" r:id="rId179" display="141984" xr:uid="{AFB539D0-83E9-4A4A-A215-13A9B804E605}"/>
+    <hyperlink ref="C148" r:id="rId180" display="142358" xr:uid="{269C2492-64F8-433D-967C-B2142FC3262F}"/>
+    <hyperlink ref="C149" r:id="rId181" display="142948" xr:uid="{9664B6F0-323A-4A90-A596-E7861D2E3800}"/>
+    <hyperlink ref="C150" r:id="rId182" display="142966" xr:uid="{F5F2CA1C-02CF-44DC-827D-F2596404CAE7}"/>
+    <hyperlink ref="C151" r:id="rId183" location="details" display="144540" xr:uid="{4BAA15E7-662D-44B6-AFDD-105E21A87787}"/>
+    <hyperlink ref="O145" r:id="rId184" xr:uid="{8B323888-0F35-4D2E-8FF6-D926B7B261B8}"/>
+    <hyperlink ref="O148" r:id="rId185" xr:uid="{3CC410BB-23BA-462C-9B06-FB0274A68A37}"/>
+    <hyperlink ref="O149" r:id="rId186" xr:uid="{D816A09A-A516-497A-847F-0D11E2C19565}"/>
+    <hyperlink ref="O150" r:id="rId187" xr:uid="{AD2121AE-D68E-4DD3-894E-45094BC647A1}"/>
+    <hyperlink ref="O147" r:id="rId188" xr:uid="{A61E4F25-C426-48DC-8D07-D3B48D120700}"/>
+    <hyperlink ref="O146" r:id="rId189" xr:uid="{927D1C8F-29E8-4CD4-8478-00D1A709F6FE}"/>
+    <hyperlink ref="O143" r:id="rId190" xr:uid="{C2B3D6F9-B05C-491A-8C42-FC583C78D5AE}"/>
+    <hyperlink ref="O142" r:id="rId191" xr:uid="{8DAF780E-E9A1-4849-9680-BF5B549882B7}"/>
+    <hyperlink ref="O141" r:id="rId192" xr:uid="{3D152074-8F00-4964-8231-4EE1D1B12ECB}"/>
+    <hyperlink ref="O139" r:id="rId193" xr:uid="{14812CAE-768F-418C-B8CA-6AA155C23D97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId172"/>
+  <pageSetup orientation="portrait" r:id="rId194"/>
   <tableParts count="1">
-    <tablePart r:id="rId173"/>
+    <tablePart r:id="rId195"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AF7F3516F12EF942A5238E40A18E1A3E" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2617042f7daf7a5562991d40a6eb3c80">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16980aa2-779a-4fd7-8eca-af4e701789d1" xmlns:ns3="7cb10c50-7b83-4937-b931-982b5a8565cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1c1757fa717c87d066a82b317eb6e9a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AF7F3516F12EF942A5238E40A18E1A3E" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="57ae05294973947ed4e2583ab1af195c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16980aa2-779a-4fd7-8eca-af4e701789d1" xmlns:ns3="7cb10c50-7b83-4937-b931-982b5a8565cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="691aecd9e3460d9c64ce3ac6e2586f0f" ns2:_="" ns3:_="">
     <xsd:import namespace="16980aa2-779a-4fd7-8eca-af4e701789d1"/>
     <xsd:import namespace="7cb10c50-7b83-4937-b931-982b5a8565cf"/>
     <xsd:element name="properties">
@@ -8481,8 +9133,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C09FF9-C6ED-4E2B-A7FA-8B2F097936F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2F4332-41C0-4CB8-A372-ACA76417C6D3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8490,7 +9157,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE31722-6D2F-44A7-87DB-AAE684E49E52}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C09FF9-C6ED-4E2B-A7FA-8B2F097936F8}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
feat: add corrective status registry and standardize unit test patterns (#14)
- Add corrective-status-registry module with full CRUD operations
  - Add 6 new monthly-report use-cases (L3 summary, incidents by day, bugs by parent, etc.)
  - Enhance analytics dashboard with comprehensive L3 analytics
  - Migrate 45+ unit tests from vi.fn() to vitest-mock-extended pattern
  - Add unit tests for categorization-registry, module-registry, and corrective-status-registry
  - Add path aliases for @categorization-registry and @module-registry

  Or a shorter version:

  feat: add corrective status registry and migrate tests to vitest-mock-extended

  - New corrective-status-registry module with CRUD operations
  - New monthly-report L3 analytics use-cases
  - Enhanced analytics dashboard
  - Standardized all unit tests to use mock<T>() and MockProxy<T>
  - Added test coverage for categorization-registry and module-registry
</commit_message>
<xml_diff>
--- a/apps/reports-api/files/EDWarRooms2025.xlsx
+++ b/apps/reports-api/files/EDWarRooms2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcorpbiz.sharepoint.com/sites/SomosBelcorpRevamp-Development/Documentos compartidos/09. Operation/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1577" documentId="11_FCBEA7B812AF3F2BC6B584C3BFED8787170E5B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB98767D-B2B3-4CD0-822F-0997C9ABF147}"/>
+  <xr:revisionPtr revIDLastSave="1815" documentId="11_FCBEA7B812AF3F2BC6B584C3BFED8787170E5B5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11DABBA-C767-4927-8421-8540E54788D4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26040" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="-120" windowWidth="26040" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warrooms" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="332">
   <si>
     <t>Application</t>
   </si>
@@ -930,6 +930,9 @@
     <t>Error by change, Resolutor changed to infra</t>
   </si>
   <si>
+    <t>https://confluence.belcorp.biz/x/MX3vDQ</t>
+  </si>
+  <si>
     <t>ALL|C16|APP CEG|BOLSA DE PEDIDO| nO se no visualizan pedidos en bolsa</t>
   </si>
   <si>
@@ -937,6 +940,102 @@
   </si>
   <si>
     <t>https://confluence.belcorp.biz/x/MxLvDQ</t>
+  </si>
+  <si>
+    <t>DO|PROL|-Error en el proceso PROL ACTIVACION BDI2</t>
+  </si>
+  <si>
+    <t>User mistake, It was identified that one of the levels of a program configured in “N per offer configuration” had a duplicate level.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/L33vDQ</t>
+  </si>
+  <si>
+    <t>MX|UNETE 2.0|BURÓ| CS sin consulta crediticia.</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>Bug, A group of zones does not keep a record of inquiries made to the credit buró and are not configured as a Cash Payment Zone.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/pyzvDQ</t>
+  </si>
+  <si>
+    <t>DO| C17| SB| Incentivos| muestra aviso a la CS que no puede seleccionar Incentivo</t>
+  </si>
+  <si>
+    <t>User mistake, Incorrect configuration of the reported contest</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/LX3vDQ</t>
+  </si>
+  <si>
+    <t>DO|C17|SB|FESTIVALES|Oferta no permite agregarse MENSAJE DE ERROR</t>
+  </si>
+  <si>
+    <t>User mistake, A double festival was set up, and the product was also sent from Affinity as part of the Festival.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/2ETvDQ</t>
+  </si>
+  <si>
+    <t>CO|C18|SB|MULTIPEDIDO POSTERIOR| No aparece experiencia de MB Posterior configurada para hoy</t>
+  </si>
+  <si>
+    <t>The ConfiguracionValidacionZona table had a value of 9 days, which was not enough to cover day 20 according to the billing start date.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/g1DvDQ</t>
+  </si>
+  <si>
+    <t>PE|C18|SB|BONIFICACIONES| NO SE PUEDE SELECCIONAR INCENTIVOS C18</t>
+  </si>
+  <si>
+    <t>Consultant identifies incorrect tender; response expected from SSICC team</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/3E3vDQ</t>
+  </si>
+  <si>
+    <t>EC|C18|SB|BONIFICACIONES|: PUNTAJE NO ACTUALIZADO</t>
+  </si>
+  <si>
+    <t>Resolutor changed to SSICC/ODS - The incentive score is not added together.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/K33vDQ</t>
+  </si>
+  <si>
+    <t>PE|C18|SB|PASE DE PEDIDOS|Producto de Televenta tiene distinto precio entre consultoras</t>
+  </si>
+  <si>
+    <t>User mistake, CUV 37043 submitted a manual update with the repetition factor at 0</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/mmfvDQ</t>
+  </si>
+  <si>
+    <t>BO|C17|PROL|PEDIDO NO SE PUEDE RESERVAR SALE ERROR CS 0721286</t>
+  </si>
+  <si>
+    <t>User mistake, The product with the internal warning has a replacement configured, which was out of stock.</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/lmfvDQ</t>
+  </si>
+  <si>
+    <t>BO|C17|SB| CS COD 0717399 NO PUEDE RESERVAR - MENSAJE DE ERROR</t>
+  </si>
+  <si>
+    <t>https://confluence.belcorp.biz/x/KX3vDQ</t>
+  </si>
+  <si>
+    <t>CR|C16|SB ADMIN|Campaña 202416 CR no disponible en somosbelcorp</t>
+  </si>
+  <si>
+    <t>Resolutor changed to SSICC/ODS -  Campaign 202416 does not exist in the records of the ods.campania table</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1148,11 +1247,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1459,8 +1564,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}" name="Tabla1" displayName="Tabla1" ref="A1:O140" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O140" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}" name="Tabla1" displayName="Tabla1" ref="A1:O152" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O152" xr:uid="{931A11FA-CC5A-4984-8426-6DB6F0FCAF03}">
+    <filterColumn colId="1">
+      <filters>
+        <dateGroupItem year="2025" month="11" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O135">
     <sortCondition ref="A1:A135"/>
   </sortState>
@@ -1804,11 +1915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O140"/>
+  <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.149999999999999" customHeight="1"/>
@@ -1884,7 +1995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="2" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -1929,7 +2040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="3" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1974,7 +2085,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="4" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2019,7 +2130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="5" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -2064,7 +2175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="6" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -2109,7 +2220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="7" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -2154,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="8" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
@@ -2199,7 +2310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="9" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -2244,7 +2355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="10" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2289,7 +2400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15" ht="15" hidden="1">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -2334,7 +2445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15">
+    <row r="12" spans="1:15" ht="15" hidden="1">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -2379,7 +2490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15">
+    <row r="13" spans="1:15" ht="15" hidden="1">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -2424,7 +2535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15">
+    <row r="14" spans="1:15" ht="15" hidden="1">
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
@@ -2469,7 +2580,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15">
+    <row r="15" spans="1:15" ht="15" hidden="1">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -2514,7 +2625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15">
+    <row r="16" spans="1:15" ht="15" hidden="1">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
@@ -2559,7 +2670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15">
+    <row r="17" spans="1:14" ht="15" hidden="1">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -2604,7 +2715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14" ht="15" hidden="1">
       <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
@@ -2649,7 +2760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="19" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15">
+    <row r="20" spans="1:14" ht="15" hidden="1">
       <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
@@ -2739,7 +2850,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="21" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
@@ -2784,7 +2895,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15">
+    <row r="22" spans="1:14" ht="15" hidden="1">
       <c r="A22" s="7" t="s">
         <v>61</v>
       </c>
@@ -2829,7 +2940,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15">
+    <row r="23" spans="1:14" ht="15" hidden="1">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2874,7 +2985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15">
+    <row r="24" spans="1:14" ht="15" hidden="1">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
@@ -2919,7 +3030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15">
+    <row r="25" spans="1:14" ht="15" hidden="1">
       <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
@@ -2964,7 +3075,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15">
+    <row r="26" spans="1:14" ht="15" hidden="1">
       <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
@@ -3009,7 +3120,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15">
+    <row r="27" spans="1:14" ht="15" hidden="1">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3054,7 +3165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="28" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
@@ -3099,7 +3210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="29" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>23</v>
       </c>
@@ -3144,7 +3255,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="30" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>61</v>
       </c>
@@ -3189,7 +3300,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="31" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>23</v>
       </c>
@@ -3234,7 +3345,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="32" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
@@ -3279,7 +3390,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="33" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
@@ -3324,7 +3435,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="34" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>23</v>
       </c>
@@ -3369,7 +3480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="35" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A35" s="7" t="s">
         <v>23</v>
       </c>
@@ -3414,7 +3525,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="36" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
@@ -3459,7 +3570,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="37" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A37" s="7" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3615,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="38" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>23</v>
       </c>
@@ -3549,7 +3660,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="39" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>15</v>
       </c>
@@ -3594,7 +3705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="40" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>23</v>
       </c>
@@ -3639,7 +3750,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="41" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>23</v>
       </c>
@@ -3684,7 +3795,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="42" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>15</v>
       </c>
@@ -3729,7 +3840,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="43" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>23</v>
       </c>
@@ -3774,7 +3885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="44" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>52</v>
       </c>
@@ -3819,7 +3930,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="45" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>15</v>
       </c>
@@ -3864,7 +3975,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="46" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>52</v>
       </c>
@@ -3909,7 +4020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="47" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
@@ -3954,7 +4065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="48" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>15</v>
       </c>
@@ -3999,7 +4110,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="49" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>23</v>
       </c>
@@ -4044,7 +4155,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="50" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>23</v>
       </c>
@@ -4089,7 +4200,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="51" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>52</v>
       </c>
@@ -4134,7 +4245,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="52" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>15</v>
       </c>
@@ -4179,7 +4290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="53" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A53" s="7" t="s">
         <v>15</v>
       </c>
@@ -4225,7 +4336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="54" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A54" s="7" t="s">
         <v>23</v>
       </c>
@@ -4270,7 +4381,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="55" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A55" s="7" t="s">
         <v>23</v>
       </c>
@@ -4315,7 +4426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="56" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A56" s="7" t="s">
         <v>15</v>
       </c>
@@ -4360,7 +4471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="57" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>23</v>
       </c>
@@ -4405,7 +4516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="58" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A58" s="7" t="s">
         <v>52</v>
       </c>
@@ -4450,7 +4561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="59" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
@@ -4495,7 +4606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="60" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A60" s="7" t="s">
         <v>23</v>
       </c>
@@ -4540,7 +4651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="61" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A61" s="7" t="s">
         <v>15</v>
       </c>
@@ -4585,7 +4696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="62" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A62" s="7" t="s">
         <v>23</v>
       </c>
@@ -4630,7 +4741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="63" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>23</v>
       </c>
@@ -4675,7 +4786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15">
+    <row r="64" spans="1:14" ht="15" hidden="1">
       <c r="A64" s="7" t="s">
         <v>23</v>
       </c>
@@ -4720,7 +4831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15">
+    <row r="65" spans="1:14" ht="15" hidden="1">
       <c r="A65" s="7" t="s">
         <v>61</v>
       </c>
@@ -4765,7 +4876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15">
+    <row r="66" spans="1:14" ht="15" hidden="1">
       <c r="A66" s="7" t="s">
         <v>23</v>
       </c>
@@ -4810,7 +4921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15">
+    <row r="67" spans="1:14" ht="15" hidden="1">
       <c r="A67" s="7" t="s">
         <v>23</v>
       </c>
@@ -4855,7 +4966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="68" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>23</v>
       </c>
@@ -4900,7 +5011,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="69" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A69" s="7" t="s">
         <v>23</v>
       </c>
@@ -4945,7 +5056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15">
+    <row r="70" spans="1:14" ht="15" hidden="1">
       <c r="A70" s="7" t="s">
         <v>23</v>
       </c>
@@ -4990,7 +5101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15">
+    <row r="71" spans="1:14" ht="15" hidden="1">
       <c r="A71" s="7" t="s">
         <v>23</v>
       </c>
@@ -5035,7 +5146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15">
+    <row r="72" spans="1:14" ht="15" hidden="1">
       <c r="A72" s="7" t="s">
         <v>23</v>
       </c>
@@ -5080,7 +5191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15">
+    <row r="73" spans="1:14" ht="15" hidden="1">
       <c r="A73" s="7" t="s">
         <v>15</v>
       </c>
@@ -5125,7 +5236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15">
+    <row r="74" spans="1:14" ht="15" hidden="1">
       <c r="A74" s="7" t="s">
         <v>23</v>
       </c>
@@ -5170,7 +5281,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15">
+    <row r="75" spans="1:14" ht="15" hidden="1">
       <c r="A75" s="7" t="s">
         <v>23</v>
       </c>
@@ -5215,7 +5326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15">
+    <row r="76" spans="1:14" ht="15" hidden="1">
       <c r="A76" s="7" t="s">
         <v>15</v>
       </c>
@@ -5260,7 +5371,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15">
+    <row r="77" spans="1:14" ht="15" hidden="1">
       <c r="A77" s="7" t="s">
         <v>15</v>
       </c>
@@ -5305,7 +5416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15">
+    <row r="78" spans="1:14" ht="15" hidden="1">
       <c r="A78" s="7" t="s">
         <v>15</v>
       </c>
@@ -5350,7 +5461,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="79" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A79" s="7" t="s">
         <v>23</v>
       </c>
@@ -5392,7 +5503,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="80" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A80" s="7" t="s">
         <v>34</v>
       </c>
@@ -5434,7 +5545,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="81" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A81" s="7" t="s">
         <v>15</v>
       </c>
@@ -5476,7 +5587,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="82" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A82" s="7" t="s">
         <v>23</v>
       </c>
@@ -5518,7 +5629,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="83" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A83" s="7" t="s">
         <v>23</v>
       </c>
@@ -5560,7 +5671,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="84" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A84" s="7" t="s">
         <v>15</v>
       </c>
@@ -5602,7 +5713,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="85" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A85" s="7" t="s">
         <v>23</v>
       </c>
@@ -5644,7 +5755,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="86" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A86" s="7" t="s">
         <v>23</v>
       </c>
@@ -5686,7 +5797,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="87" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A87" s="7" t="s">
         <v>23</v>
       </c>
@@ -5728,7 +5839,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="88" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A88" s="18" t="s">
         <v>23</v>
       </c>
@@ -5770,7 +5881,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="89" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A89" s="18" t="s">
         <v>23</v>
       </c>
@@ -5812,7 +5923,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="90" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A90" s="7" t="s">
         <v>15</v>
       </c>
@@ -5854,7 +5965,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="91" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A91" s="7" t="s">
         <v>15</v>
       </c>
@@ -5896,7 +6007,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="92" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A92" s="7" t="s">
         <v>15</v>
       </c>
@@ -5938,7 +6049,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="93" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A93" s="18" t="s">
         <v>23</v>
       </c>
@@ -5980,7 +6091,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="94" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A94" s="7" t="s">
         <v>15</v>
       </c>
@@ -6022,7 +6133,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="95" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A95" s="18" t="s">
         <v>23</v>
       </c>
@@ -6064,7 +6175,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="16.149999999999999" customHeight="1">
+    <row r="96" spans="1:13" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A96" s="18" t="s">
         <v>23</v>
       </c>
@@ -6106,7 +6217,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="97" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A97" s="18" t="s">
         <v>23</v>
       </c>
@@ -6148,7 +6259,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="98" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A98" s="18" t="s">
         <v>23</v>
       </c>
@@ -6190,7 +6301,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="99" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A99" s="18" t="s">
         <v>23</v>
       </c>
@@ -6232,7 +6343,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="100" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A100" s="18" t="s">
         <v>34</v>
       </c>
@@ -6274,7 +6385,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="101" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A101" s="18" t="s">
         <v>23</v>
       </c>
@@ -6316,7 +6427,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="102" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A102" s="18" t="s">
         <v>23</v>
       </c>
@@ -6358,7 +6469,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="16.149999999999999" customHeight="1">
+    <row r="103" spans="1:14" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A103" s="18" t="s">
         <v>34</v>
       </c>
@@ -6400,7 +6511,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15">
+    <row r="104" spans="1:14" ht="15" hidden="1">
       <c r="A104" s="18" t="s">
         <v>23</v>
       </c>
@@ -6442,7 +6553,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="15">
+    <row r="105" spans="1:14" ht="15" hidden="1">
       <c r="A105" s="18" t="s">
         <v>23</v>
       </c>
@@ -6484,7 +6595,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="15">
+    <row r="106" spans="1:14" ht="15" hidden="1">
       <c r="A106" s="18" t="s">
         <v>23</v>
       </c>
@@ -6526,7 +6637,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="15">
+    <row r="107" spans="1:14" ht="15" hidden="1">
       <c r="A107" s="18" t="s">
         <v>23</v>
       </c>
@@ -6568,7 +6679,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15">
+    <row r="108" spans="1:14" ht="15" hidden="1">
       <c r="A108" s="18" t="s">
         <v>23</v>
       </c>
@@ -6610,7 +6721,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15">
+    <row r="109" spans="1:14" ht="15" hidden="1">
       <c r="A109" s="7" t="s">
         <v>15</v>
       </c>
@@ -6652,7 +6763,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="15">
+    <row r="110" spans="1:14" ht="15" hidden="1">
       <c r="A110" s="18" t="s">
         <v>34</v>
       </c>
@@ -6694,7 +6805,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15">
+    <row r="111" spans="1:14" ht="15" hidden="1">
       <c r="A111" s="7" t="s">
         <v>15</v>
       </c>
@@ -6739,7 +6850,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="15">
+    <row r="112" spans="1:14" ht="15" hidden="1">
       <c r="A112" s="18" t="s">
         <v>23</v>
       </c>
@@ -6784,7 +6895,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="15">
+    <row r="113" spans="1:15" ht="15" hidden="1">
       <c r="A113" s="18" t="s">
         <v>23</v>
       </c>
@@ -6832,7 +6943,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="15">
+    <row r="114" spans="1:15" ht="15" hidden="1">
       <c r="A114" s="18" t="s">
         <v>23</v>
       </c>
@@ -6877,7 +6988,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="15">
+    <row r="115" spans="1:15" ht="15" hidden="1">
       <c r="A115" s="18" t="s">
         <v>23</v>
       </c>
@@ -6922,7 +7033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="15">
+    <row r="116" spans="1:15" ht="15" hidden="1">
       <c r="A116" s="18" t="s">
         <v>23</v>
       </c>
@@ -6967,7 +7078,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="117" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A117" s="18" t="s">
         <v>23</v>
       </c>
@@ -7015,7 +7126,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="15">
+    <row r="118" spans="1:15" ht="15" hidden="1">
       <c r="A118" s="7" t="s">
         <v>15</v>
       </c>
@@ -7063,7 +7174,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="15">
+    <row r="119" spans="1:15" ht="15" hidden="1">
       <c r="A119" s="7" t="s">
         <v>15</v>
       </c>
@@ -7108,7 +7219,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="15">
+    <row r="120" spans="1:15" ht="15" hidden="1">
       <c r="A120" s="30" t="s">
         <v>23</v>
       </c>
@@ -7156,7 +7267,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="15">
+    <row r="121" spans="1:15" ht="15" hidden="1">
       <c r="A121" s="30" t="s">
         <v>23</v>
       </c>
@@ -7201,7 +7312,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="15">
+    <row r="122" spans="1:15" ht="15" hidden="1">
       <c r="A122" s="18" t="s">
         <v>23</v>
       </c>
@@ -7246,7 +7357,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="123" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A123" s="28" t="s">
         <v>251</v>
       </c>
@@ -7294,7 +7405,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="124" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A124" s="7" t="s">
         <v>15</v>
       </c>
@@ -7342,7 +7453,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="15">
+    <row r="125" spans="1:15" ht="15" hidden="1">
       <c r="A125" s="7" t="s">
         <v>15</v>
       </c>
@@ -7390,7 +7501,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="126" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A126" s="7" t="s">
         <v>15</v>
       </c>
@@ -7435,7 +7546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="127" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A127" s="18" t="s">
         <v>23</v>
       </c>
@@ -7483,7 +7594,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="128" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A128" s="18" t="s">
         <v>23</v>
       </c>
@@ -7531,7 +7642,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="129" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A129" s="18" t="s">
         <v>23</v>
       </c>
@@ -7541,7 +7652,7 @@
       <c r="C129" s="36">
         <v>128089</v>
       </c>
-      <c r="D129" s="41" t="s">
+      <c r="D129" s="40" t="s">
         <v>270</v>
       </c>
       <c r="E129" s="7" t="s">
@@ -7579,7 +7690,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="130" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A130" s="18" t="s">
         <v>23</v>
       </c>
@@ -7627,7 +7738,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="131" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A131" s="18" t="s">
         <v>23</v>
       </c>
@@ -7672,7 +7783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="132" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A132" s="18" t="s">
         <v>23</v>
       </c>
@@ -7717,7 +7828,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="133" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A133" s="18" t="s">
         <v>23</v>
       </c>
@@ -7765,7 +7876,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="134" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A134" s="28" t="s">
         <v>23</v>
       </c>
@@ -7810,7 +7921,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="135" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A135" s="18" t="s">
         <v>34</v>
       </c>
@@ -7855,11 +7966,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="136" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A136" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B136" s="40">
+      <c r="B136" s="19">
         <v>45958</v>
       </c>
       <c r="C136" s="36">
@@ -7900,11 +8011,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="137" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A137" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B137" s="40">
+      <c r="B137" s="19">
         <v>45958</v>
       </c>
       <c r="C137" s="36">
@@ -7945,11 +8056,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="16.149999999999999" customHeight="1">
+    <row r="138" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
       <c r="A138" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B138" s="40">
+      <c r="B138" s="19">
         <v>45958</v>
       </c>
       <c r="C138" s="36">
@@ -7994,7 +8105,7 @@
       <c r="A139" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B139" s="40">
+      <c r="B139" s="19">
         <v>45965</v>
       </c>
       <c r="C139" s="36">
@@ -8033,20 +8144,23 @@
       </c>
       <c r="N139" s="7" t="s">
         <v>46</v>
+      </c>
+      <c r="O139" s="26" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16.149999999999999" customHeight="1">
       <c r="A140" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B140" s="40">
+      <c r="B140" s="19">
         <v>45966</v>
       </c>
       <c r="C140" s="36">
         <v>136341</v>
       </c>
       <c r="D140" s="35" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>17</v>
@@ -8074,14 +8188,545 @@
         <v>20</v>
       </c>
       <c r="M140" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N140" s="7" t="s">
         <v>221</v>
       </c>
       <c r="O140" s="26" t="s">
-        <v>298</v>
-      </c>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A141" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="19">
+        <v>45971</v>
+      </c>
+      <c r="C141" s="36">
+        <v>137357</v>
+      </c>
+      <c r="D141" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" s="10">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="G141" s="7">
+        <v>105</v>
+      </c>
+      <c r="H141" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="I141" s="7">
+        <v>7</v>
+      </c>
+      <c r="J141" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K141" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L141" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M141" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="N141" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O141" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A142" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B142" s="19">
+        <v>45973</v>
+      </c>
+      <c r="C142" s="36">
+        <v>138367</v>
+      </c>
+      <c r="D142" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="E142" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F142" s="10">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="G142" s="7">
+        <v>240</v>
+      </c>
+      <c r="H142" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="I142" s="7">
+        <v>15</v>
+      </c>
+      <c r="J142" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K142" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L142" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M142" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="N142" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O142" s="26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A143" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B143" s="19">
+        <v>45974</v>
+      </c>
+      <c r="C143" s="41">
+        <v>138895</v>
+      </c>
+      <c r="D143" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F143" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G143" s="7">
+        <v>150</v>
+      </c>
+      <c r="H143" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="I143" s="7">
+        <v>6</v>
+      </c>
+      <c r="J143" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L143" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M143" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="N143" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O143" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A144" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" s="19">
+        <v>45981</v>
+      </c>
+      <c r="C144" s="36">
+        <v>139556</v>
+      </c>
+      <c r="D144" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F144" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G144" s="7">
+        <v>160</v>
+      </c>
+      <c r="H144" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="I144" s="7">
+        <v>9</v>
+      </c>
+      <c r="J144" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K144" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L144" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M144" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="N144" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O144" s="37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A145" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B145" s="19">
+        <v>45981</v>
+      </c>
+      <c r="C145" s="36">
+        <v>140551</v>
+      </c>
+      <c r="D145" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F145" s="10">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="G145" s="7">
+        <v>210</v>
+      </c>
+      <c r="H145" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.76388888888888895</v>
+      </c>
+      <c r="I145" s="7">
+        <v>13</v>
+      </c>
+      <c r="J145" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M145" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="N145" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O145" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A146" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B146" s="19">
+        <v>45985</v>
+      </c>
+      <c r="C146" s="36">
+        <v>141251</v>
+      </c>
+      <c r="D146" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F146" s="10">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="G146" s="7">
+        <v>175</v>
+      </c>
+      <c r="H146" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.53125</v>
+      </c>
+      <c r="I146" s="7">
+        <v>12</v>
+      </c>
+      <c r="J146" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K146" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L146" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M146" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="N146" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O146" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A147" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" s="19">
+        <v>45986</v>
+      </c>
+      <c r="C147" s="36">
+        <v>141984</v>
+      </c>
+      <c r="D147" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F147" s="10">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G147" s="7">
+        <v>50</v>
+      </c>
+      <c r="H147" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.83680555555555558</v>
+      </c>
+      <c r="I147" s="7">
+        <v>5</v>
+      </c>
+      <c r="J147" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K147" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L147" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M147" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="N147" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O147" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A148" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B148" s="42">
+        <v>45987</v>
+      </c>
+      <c r="C148" s="36">
+        <v>142358</v>
+      </c>
+      <c r="D148" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F148" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G148" s="7">
+        <v>50</v>
+      </c>
+      <c r="H148" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="I148" s="7">
+        <v>4</v>
+      </c>
+      <c r="J148" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K148" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L148" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M148" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="N148" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O148" s="26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A149" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B149" s="42">
+        <v>45989</v>
+      </c>
+      <c r="C149" s="36">
+        <v>142948</v>
+      </c>
+      <c r="D149" t="s">
+        <v>325</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F149" s="10">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G149" s="7">
+        <v>70</v>
+      </c>
+      <c r="H149" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I149" s="7">
+        <v>6</v>
+      </c>
+      <c r="J149" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M149" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N149" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="O149" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" ht="16.149999999999999" customHeight="1">
+      <c r="A150" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B150" s="42">
+        <v>45989</v>
+      </c>
+      <c r="C150" s="36">
+        <v>142966</v>
+      </c>
+      <c r="D150" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F150" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G150" s="7">
+        <v>65</v>
+      </c>
+      <c r="H150" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="I150" s="7">
+        <v>8</v>
+      </c>
+      <c r="J150" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L150" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M150" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N150" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O150" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
+      <c r="A151" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="42">
+        <v>45994</v>
+      </c>
+      <c r="C151" s="36">
+        <v>144540</v>
+      </c>
+      <c r="D151" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F151" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="G151" s="7">
+        <v>35</v>
+      </c>
+      <c r="H151" s="10">
+        <f>Tabla1[[#This Row],[Start Time]]+(Tabla1[[#This Row],[Duration (Minutes)]]/1440)</f>
+        <v>0.71180555555555558</v>
+      </c>
+      <c r="I151" s="7">
+        <v>12</v>
+      </c>
+      <c r="J151" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K151" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M151" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="N151" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="16.149999999999999" hidden="1" customHeight="1">
+      <c r="A152" s="28"/>
+      <c r="B152" s="42"/>
+      <c r="C152" s="43"/>
+      <c r="F152" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8256,33 +8901,40 @@
     <hyperlink ref="C139" r:id="rId169" display="136040" xr:uid="{F80D565B-B60C-432B-B5E5-A8D4B680A58A}"/>
     <hyperlink ref="C140" r:id="rId170" display="136341" xr:uid="{A2DA186D-87E9-49EB-A8D4-844EFEF3E0BC}"/>
     <hyperlink ref="O140" r:id="rId171" xr:uid="{73E6D2D9-56BF-485D-AC48-A46E59BCA29A}"/>
+    <hyperlink ref="C141" r:id="rId172" display="137357" xr:uid="{641393F9-91E6-41F8-9FC9-AEF2EB5CCFA5}"/>
+    <hyperlink ref="C142" r:id="rId173" display="138367" xr:uid="{0BBFBABF-045E-43A3-9668-881698CD6281}"/>
+    <hyperlink ref="C143" r:id="rId174" display="138895" xr:uid="{5E323059-89CB-4C7C-A1B3-B288E2F62593}"/>
+    <hyperlink ref="C144" r:id="rId175" display="139556" xr:uid="{8B91B6CF-93A5-471F-9B80-6E3CE24578C0}"/>
+    <hyperlink ref="O144" r:id="rId176" xr:uid="{0815C2D1-F220-4592-9369-C67917B4D98F}"/>
+    <hyperlink ref="C145" r:id="rId177" display="140551" xr:uid="{374FBAB6-0BA4-4063-9DAC-8FB8296334B4}"/>
+    <hyperlink ref="C146" r:id="rId178" display="141251" xr:uid="{0BF9A3AC-0A07-4ABE-83F2-7BAE5BBE750B}"/>
+    <hyperlink ref="C147" r:id="rId179" display="141984" xr:uid="{AFB539D0-83E9-4A4A-A215-13A9B804E605}"/>
+    <hyperlink ref="C148" r:id="rId180" display="142358" xr:uid="{269C2492-64F8-433D-967C-B2142FC3262F}"/>
+    <hyperlink ref="C149" r:id="rId181" display="142948" xr:uid="{9664B6F0-323A-4A90-A596-E7861D2E3800}"/>
+    <hyperlink ref="C150" r:id="rId182" display="142966" xr:uid="{F5F2CA1C-02CF-44DC-827D-F2596404CAE7}"/>
+    <hyperlink ref="C151" r:id="rId183" location="details" display="144540" xr:uid="{4BAA15E7-662D-44B6-AFDD-105E21A87787}"/>
+    <hyperlink ref="O145" r:id="rId184" xr:uid="{8B323888-0F35-4D2E-8FF6-D926B7B261B8}"/>
+    <hyperlink ref="O148" r:id="rId185" xr:uid="{3CC410BB-23BA-462C-9B06-FB0274A68A37}"/>
+    <hyperlink ref="O149" r:id="rId186" xr:uid="{D816A09A-A516-497A-847F-0D11E2C19565}"/>
+    <hyperlink ref="O150" r:id="rId187" xr:uid="{AD2121AE-D68E-4DD3-894E-45094BC647A1}"/>
+    <hyperlink ref="O147" r:id="rId188" xr:uid="{A61E4F25-C426-48DC-8D07-D3B48D120700}"/>
+    <hyperlink ref="O146" r:id="rId189" xr:uid="{927D1C8F-29E8-4CD4-8478-00D1A709F6FE}"/>
+    <hyperlink ref="O143" r:id="rId190" xr:uid="{C2B3D6F9-B05C-491A-8C42-FC583C78D5AE}"/>
+    <hyperlink ref="O142" r:id="rId191" xr:uid="{8DAF780E-E9A1-4849-9680-BF5B549882B7}"/>
+    <hyperlink ref="O141" r:id="rId192" xr:uid="{3D152074-8F00-4964-8231-4EE1D1B12ECB}"/>
+    <hyperlink ref="O139" r:id="rId193" xr:uid="{14812CAE-768F-418C-B8CA-6AA155C23D97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId172"/>
+  <pageSetup orientation="portrait" r:id="rId194"/>
   <tableParts count="1">
-    <tablePart r:id="rId173"/>
+    <tablePart r:id="rId195"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AF7F3516F12EF942A5238E40A18E1A3E" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2617042f7daf7a5562991d40a6eb3c80">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16980aa2-779a-4fd7-8eca-af4e701789d1" xmlns:ns3="7cb10c50-7b83-4937-b931-982b5a8565cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1c1757fa717c87d066a82b317eb6e9a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AF7F3516F12EF942A5238E40A18E1A3E" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="57ae05294973947ed4e2583ab1af195c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16980aa2-779a-4fd7-8eca-af4e701789d1" xmlns:ns3="7cb10c50-7b83-4937-b931-982b5a8565cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="691aecd9e3460d9c64ce3ac6e2586f0f" ns2:_="" ns3:_="">
     <xsd:import namespace="16980aa2-779a-4fd7-8eca-af4e701789d1"/>
     <xsd:import namespace="7cb10c50-7b83-4937-b931-982b5a8565cf"/>
     <xsd:element name="properties">
@@ -8481,8 +9133,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C09FF9-C6ED-4E2B-A7FA-8B2F097936F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2F4332-41C0-4CB8-A372-ACA76417C6D3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8490,7 +9157,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE31722-6D2F-44A7-87DB-AAE684E49E52}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C09FF9-C6ED-4E2B-A7FA-8B2F097936F8}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>